<commit_message>
Sequelize model talking to database. Trying to sort out join
</commit_message>
<xml_diff>
--- a/documentation/Fathom Copy of Financial_Import_-_Monthly.xlsx
+++ b/documentation/Fathom Copy of Financial_Import_-_Monthly.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njbil\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\MTUCAN9Z\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\njbil\ND Office Echo\AU-895H5UH5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="114">
   <si>
     <t>Company Name:</t>
   </si>
@@ -307,30 +307,15 @@
     <t>5-502000</t>
   </si>
   <si>
-    <t>Trade &amp; Professional Creditors</t>
-  </si>
-  <si>
     <t>2-222000</t>
   </si>
   <si>
-    <t>Payroll Creditors</t>
-  </si>
-  <si>
-    <t>Tax Creditors</t>
-  </si>
-  <si>
     <t>2-224000</t>
   </si>
   <si>
     <t>Other Creditors</t>
   </si>
   <si>
-    <t>2-225100</t>
-  </si>
-  <si>
-    <t>2-225200</t>
-  </si>
-  <si>
     <t>Provisions</t>
   </si>
   <si>
@@ -350,6 +335,33 @@
   </si>
   <si>
     <t>IA</t>
+  </si>
+  <si>
+    <t>All Creditors</t>
+  </si>
+  <si>
+    <t>Payroll Liabilites</t>
+  </si>
+  <si>
+    <t>GST Liabilities</t>
+  </si>
+  <si>
+    <t>2-225000</t>
+  </si>
+  <si>
+    <t>Income Tax Payable</t>
+  </si>
+  <si>
+    <t>2-231100</t>
+  </si>
+  <si>
+    <t>2-231200</t>
+  </si>
+  <si>
+    <t>5-510000</t>
+  </si>
+  <si>
+    <t>To be determined</t>
   </si>
 </sst>
 </file>
@@ -373,7 +385,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +416,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -417,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -461,6 +485,23 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +1025,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>72</v>
@@ -1031,7 +1072,7 @@
         <v>73</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
@@ -1045,10 +1086,10 @@
         <v>34</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -1065,7 +1106,7 @@
         <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -1079,10 +1120,10 @@
         <v>35</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
@@ -1092,7 +1133,15 @@
       <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
+      <c r="A20" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>109</v>
+      </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -1101,13 +1150,7 @@
       <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -1117,13 +1160,11 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>49</v>
+        <v>5</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
@@ -1134,13 +1175,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>102</v>
+        <v>37</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>110</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
@@ -1150,7 +1191,15 @@
       <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
+      <c r="A24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>98</v>
+      </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
@@ -1159,13 +1208,7 @@
       <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="B25" s="11"/>
-      <c r="C25" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
@@ -1175,13 +1218,11 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>40</v>
+        <v>5</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -1192,13 +1233,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -1208,7 +1249,15 @@
       <c r="I27" s="9"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
+      <c r="A28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
@@ -1217,42 +1266,34 @@
       <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="6" t="s">
-        <v>6</v>
-      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
+        <v>5</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -1264,12 +1305,12 @@
         <v>7</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="D32" s="1"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
@@ -1277,7 +1318,15 @@
       <c r="I32" s="9"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="11"/>
+      <c r="A33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>46</v>
+      </c>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
@@ -1286,13 +1335,7 @@
       <c r="I33" s="9"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="B34" s="11"/>
-      <c r="C34" s="6" t="s">
-        <v>12</v>
-      </c>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
@@ -1302,13 +1345,11 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -1335,7 +1376,15 @@
       <c r="I36" s="9"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="11"/>
+      <c r="A37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
@@ -1345,9 +1394,6 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B38" s="11"/>
-      <c r="C38" s="6" t="s">
-        <v>81</v>
-      </c>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
@@ -1356,13 +1402,8 @@
       <c r="I38" s="9"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="14" t="s">
+      <c r="B39" s="11"/>
+      <c r="C39" s="6" t="s">
         <v>81</v>
       </c>
       <c r="D39" s="9"/>
@@ -1373,7 +1414,15 @@
       <c r="I39" s="9"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="11"/>
+      <c r="A40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>81</v>
+      </c>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
@@ -1383,9 +1432,6 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B41" s="11"/>
-      <c r="C41" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
@@ -1394,13 +1440,8 @@
       <c r="I41" s="9"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="8" t="s">
+      <c r="B42" s="11"/>
+      <c r="C42" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D42" s="9"/>
@@ -1411,7 +1452,15 @@
       <c r="I42" s="9"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="11"/>
+      <c r="A43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
@@ -1420,13 +1469,7 @@
       <c r="I43" s="9"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="B44" s="11"/>
-      <c r="C44" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
@@ -1436,12 +1479,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="11"/>
+      <c r="C45" s="6" t="s">
         <v>70</v>
       </c>
       <c r="D45" s="9"/>
@@ -1452,7 +1493,15 @@
       <c r="I45" s="9"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="11"/>
+      <c r="A46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>70</v>
+      </c>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
@@ -1461,13 +1510,7 @@
       <c r="I46" s="9"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="B47" s="11"/>
-      <c r="C47" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
@@ -1477,13 +1520,11 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>92</v>
+        <v>5</v>
+      </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="9"/>
@@ -1497,10 +1538,10 @@
         <v>10</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>83</v>
+        <v>93</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="9"/>
@@ -1514,10 +1555,10 @@
         <v>10</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>11</v>
+        <v>84</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="9"/>
@@ -1531,10 +1572,10 @@
         <v>10</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
@@ -1548,10 +1589,10 @@
         <v>10</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
@@ -1565,10 +1606,10 @@
         <v>10</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="9"/>
@@ -1578,7 +1619,15 @@
       <c r="I53" s="9"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="11"/>
+      <c r="A54" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="D54" s="9"/>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
@@ -1587,12 +1636,14 @@
       <c r="I54" s="9"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="6" t="s">
-        <v>16</v>
+      <c r="A55" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B55" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C55" s="23" t="s">
+        <v>113</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="9"/>
@@ -1603,16 +1654,20 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B56" s="11"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="B57" s="11"/>
+      <c r="C57" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9"/>
@@ -1623,18 +1678,32 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B58" s="11"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="11"/>
+      <c r="A59" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B60" s="11"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B61" s="11"/>
@@ -1767,6 +1836,12 @@
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="11"/>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105" s="11"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1775,17 +1850,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5042EC-0437-4F49-B1F0-F4B221559A7F}">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="15.7109375" customWidth="1"/>
+    <col min="3" max="12" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -1812,46 +1887,61 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="20">
         <v>41821</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="21">
         <v>41852</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="21">
         <v>41883</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="21">
         <v>41913</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="21">
         <v>41944</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="21">
         <v>41974</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>60</v>
       </c>
+      <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>50</v>
       </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
     </row>
     <row r="8" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>51</v>
       </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
@@ -1896,7 +1986,7 @@
     </row>
     <row r="18" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1936,7 +2026,7 @@
     </row>
     <row r="26" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1944,7 +2034,7 @@
     <row r="29" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="13" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1957,7 +2047,6 @@
     <row r="37" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="38" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="39" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>